<commit_message>
update new method to generate png
</commit_message>
<xml_diff>
--- a/dataset/circle/pattern_parameters.xlsx
+++ b/dataset/circle/pattern_parameters.xlsx
@@ -476,7 +476,7 @@
         <v>200</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="3">
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>60</v>
+        <v>61.11111111111111</v>
       </c>
       <c r="C3" t="n">
         <v>200</v>
@@ -495,7 +495,7 @@
         <v>200</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="4">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>72</v>
+        <v>72.22222222222223</v>
       </c>
       <c r="C4" t="n">
         <v>200</v>
@@ -514,7 +514,7 @@
         <v>200</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>82</v>
+        <v>83.33333333333333</v>
       </c>
       <c r="C5" t="n">
         <v>200</v>
@@ -533,7 +533,7 @@
         <v>200</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>94</v>
+        <v>94.44444444444444</v>
       </c>
       <c r="C6" t="n">
         <v>200</v>
@@ -552,7 +552,7 @@
         <v>200</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>104</v>
+        <v>105.5555555555556</v>
       </c>
       <c r="C7" t="n">
         <v>200</v>
@@ -571,7 +571,7 @@
         <v>200</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8">
@@ -581,7 +581,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>116</v>
+        <v>116.6666666666667</v>
       </c>
       <c r="C8" t="n">
         <v>200</v>
@@ -590,7 +590,7 @@
         <v>200</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="9">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>126</v>
+        <v>127.7777777777778</v>
       </c>
       <c r="C9" t="n">
         <v>200</v>
@@ -609,7 +609,7 @@
         <v>200</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="10">
@@ -619,7 +619,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>138</v>
+        <v>138.8888888888889</v>
       </c>
       <c r="C10" t="n">
         <v>200</v>
@@ -628,7 +628,7 @@
         <v>200</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="11">
@@ -647,7 +647,7 @@
         <v>200</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>